<commit_message>
Updated spmm.project and auto.spmm
</commit_message>
<xml_diff>
--- a/misc/spmm-workbook-template.xlsx
+++ b/misc/spmm-workbook-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caldridge\Documents\R\meta-pop-bio\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/caleb_aldridge_fws_gov/Documents/Documents/R/meta-pop-bio/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9677A2D-E047-4967-890B-DAD21CA56255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C9677A2D-E047-4967-890B-DAD21CA56255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0F16310-EDA6-4828-A031-57E4528F48E1}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>n_stages</t>
   </si>
@@ -101,6 +101,35 @@
   </si>
   <si>
     <t>Please see spmm example workbook for additional guidance.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">N </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>by stages</t>
+    </r>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -132,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,33 +234,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -519,57 +566,89 @@
     <col min="1" max="1" width="13.734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.26171875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83984375" style="2"/>
-    <col min="4" max="4" width="77.9453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1"/>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -579,8 +658,21 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="D4:K4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Begin building the spmm.readxl function vignette
</commit_message>
<xml_diff>
--- a/misc/spmm-workbook-template.xlsx
+++ b/misc/spmm-workbook-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/caleb_aldridge_fws_gov/Documents/Documents/R/meta-pop-bio/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C9677A2D-E047-4967-890B-DAD21CA56255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0F16310-EDA6-4828-A031-57E4528F48E1}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{C9677A2D-E047-4967-890B-DAD21CA56255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27728301-6E30-442B-ADE3-6FE8B01F5308}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -223,17 +223,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -251,30 +240,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,6 +395,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -569,110 +678,107 @@
     <col min="4" max="5" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1"/>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="D1" s="5"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="15" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="D4:K4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>